<commit_message>
updated possible column read error in aggregate_spp_ranges; wrapping up hotspot exploration but need to rerun the species lists
</commit_message>
<xml_diff>
--- a/data_explore/cells_to_explore.xlsx
+++ b/data_explore/cells_to_explore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="10000" yWindow="800" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>cell_id</t>
   </si>
   <si>
-    <t>group_name</t>
-  </si>
-  <si>
     <t>alaska</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>n_sea_of_cortez</t>
   </si>
   <si>
-    <t>philippines</t>
-  </si>
-  <si>
     <t>w_madagascar</t>
   </si>
   <si>
@@ -60,15 +54,9 @@
     <t>galapagos</t>
   </si>
   <si>
-    <t>orkney</t>
-  </si>
-  <si>
     <t>fiji</t>
   </si>
   <si>
-    <t>andamans</t>
-  </si>
-  <si>
     <t>med_a</t>
   </si>
   <si>
@@ -79,6 +67,18 @@
   </si>
   <si>
     <t>black_sea</t>
+  </si>
+  <si>
+    <t>cell_group</t>
+  </si>
+  <si>
+    <t>e_indian_ocean</t>
+  </si>
+  <si>
+    <t>faeroe</t>
+  </si>
+  <si>
+    <t>papua_new_guinea</t>
   </si>
 </sst>
 </file>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -468,7 +468,7 @@
         <v>1116276</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -476,7 +476,7 @@
         <v>1062285</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -484,7 +484,7 @@
         <v>1127083</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -492,7 +492,7 @@
         <v>4827640</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -500,7 +500,7 @@
         <v>4838443</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -508,7 +508,7 @@
         <v>4849246</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -516,7 +516,7 @@
         <v>4892449</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -524,7 +524,7 @@
         <v>1930166</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -532,7 +532,7 @@
         <v>1926570</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -540,7 +540,7 @@
         <v>1919372</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -548,7 +548,7 @@
         <v>1915782</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -556,7 +556,7 @@
         <v>2200221</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -564,7 +564,7 @@
         <v>2200230</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -572,7 +572,7 @@
         <v>2203835</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -580,7 +580,7 @@
         <v>2211043</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -588,7 +588,7 @@
         <v>2221857</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -596,7 +596,7 @@
         <v>2110256</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -604,7 +604,7 @@
         <v>2124660</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -612,7 +612,7 @@
         <v>3398131</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -620,7 +620,7 @@
         <v>3398132</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -628,7 +628,7 @@
         <v>3398133</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -636,7 +636,7 @@
         <v>4045004</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -644,7 +644,7 @@
         <v>4048604</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -652,7 +652,7 @@
         <v>3969436</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -660,7 +660,7 @@
         <v>3965838</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -668,7 +668,7 @@
         <v>3944241</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -676,7 +676,7 @@
         <v>4012758</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -684,7 +684,7 @@
         <v>4009158</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -692,7 +692,7 @@
         <v>3973169</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -700,7 +700,7 @@
         <v>3973171</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -708,7 +708,7 @@
         <v>4577279</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -716,7 +716,7 @@
         <v>4584479</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -724,7 +724,7 @@
         <v>4616886</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -732,7 +732,7 @@
         <v>5098711</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -740,7 +740,7 @@
         <v>5098712</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -748,7 +748,7 @@
         <v>3248104</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -756,7 +756,7 @@
         <v>3273298</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -764,7 +764,7 @@
         <v>3284111</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -772,7 +772,7 @@
         <v>3330885</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -780,7 +780,7 @@
         <v>1045794</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -788,7 +788,7 @@
         <v>1009795</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -796,7 +796,7 @@
         <v>962997</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -804,7 +804,7 @@
         <v>941395</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -812,7 +812,7 @@
         <v>3877173</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -820,7 +820,7 @@
         <v>3884370</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -828,7 +828,7 @@
         <v>3880763</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -836,7 +836,7 @@
         <v>3170683</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -844,7 +844,7 @@
         <v>3152735</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -852,7 +852,7 @@
         <v>3152756</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -860,7 +860,7 @@
         <v>3145557</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -868,7 +868,7 @@
         <v>1927804</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -876,7 +876,7 @@
         <v>1909858</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -884,7 +884,7 @@
         <v>1873899</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -892,7 +892,7 @@
         <v>1899096</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -900,7 +900,7 @@
         <v>1891894</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -908,7 +908,7 @@
         <v>1935136</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -916,7 +916,7 @@
         <v>1949546</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -924,7 +924,7 @@
         <v>1942349</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -932,7 +932,7 @@
         <v>1658165</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -940,7 +940,7 @@
         <v>1632967</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up a data explore to map points of interest; still need to get a data table to show up.  Maybe convert to shiny app?
</commit_message>
<xml_diff>
--- a/data_explore/cells_to_explore.xlsx
+++ b/data_explore/cells_to_explore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10000" yWindow="800" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,71 +24,87 @@
     <t>cell_id</t>
   </si>
   <si>
-    <t>alaska</t>
-  </si>
-  <si>
-    <t>se_of_nz</t>
-  </si>
-  <si>
-    <t>monterey_bay</t>
-  </si>
-  <si>
-    <t>vizcaino_bay</t>
-  </si>
-  <si>
-    <t>n_sea_of_cortez</t>
-  </si>
-  <si>
-    <t>w_madagascar</t>
-  </si>
-  <si>
-    <t>reunion</t>
-  </si>
-  <si>
-    <t>tristan_da_cunha</t>
-  </si>
-  <si>
-    <t>tierra_del_fuego</t>
-  </si>
-  <si>
-    <t>galapagos</t>
-  </si>
-  <si>
-    <t>fiji</t>
-  </si>
-  <si>
-    <t>med_a</t>
-  </si>
-  <si>
-    <t>med_b</t>
-  </si>
-  <si>
-    <t>med_c</t>
-  </si>
-  <si>
-    <t>black_sea</t>
-  </si>
-  <si>
     <t>cell_group</t>
   </si>
   <si>
-    <t>e_indian_ocean</t>
-  </si>
-  <si>
-    <t>faeroe</t>
-  </si>
-  <si>
-    <t>papua_new_guinea</t>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>New Zealand SE</t>
+  </si>
+  <si>
+    <t>Monterey Bay</t>
+  </si>
+  <si>
+    <t>Vizcaino Bay Baja</t>
+  </si>
+  <si>
+    <t>N Sea of Cortez</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>W Madagascar</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Tristan da Cunha</t>
+  </si>
+  <si>
+    <t>Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Galapagos</t>
+  </si>
+  <si>
+    <t>Faeroe Islands</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Black Sea</t>
+  </si>
+  <si>
+    <t>Mediterranean Sea 1</t>
+  </si>
+  <si>
+    <t>Mediterranean Sea 2</t>
+  </si>
+  <si>
+    <t>Mediterranean Sea 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,13 +127,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -460,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -468,7 +496,7 @@
         <v>1116276</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -476,7 +504,7 @@
         <v>1062285</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -484,7 +512,7 @@
         <v>1127083</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -492,7 +520,7 @@
         <v>4827640</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -500,7 +528,7 @@
         <v>4838443</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -508,7 +536,7 @@
         <v>4849246</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -516,7 +544,7 @@
         <v>4892449</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -524,7 +552,7 @@
         <v>1930166</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -532,7 +560,7 @@
         <v>1926570</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -540,7 +568,7 @@
         <v>1919372</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -548,7 +576,7 @@
         <v>1915782</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -556,7 +584,7 @@
         <v>2200221</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -564,7 +592,7 @@
         <v>2200230</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -572,7 +600,7 @@
         <v>2203835</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -580,7 +608,7 @@
         <v>2211043</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -588,7 +616,7 @@
         <v>2221857</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -596,7 +624,7 @@
         <v>2110256</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -604,7 +632,7 @@
         <v>2124660</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -612,7 +640,7 @@
         <v>3398131</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -620,7 +648,7 @@
         <v>3398132</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -628,7 +656,7 @@
         <v>3398133</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -636,7 +664,7 @@
         <v>4045004</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -644,7 +672,7 @@
         <v>4048604</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -652,7 +680,7 @@
         <v>3969436</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -660,7 +688,7 @@
         <v>3965838</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -668,7 +696,7 @@
         <v>3944241</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -676,7 +704,7 @@
         <v>4012758</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -684,7 +712,7 @@
         <v>4009158</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -692,7 +720,7 @@
         <v>3973169</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -700,7 +728,7 @@
         <v>3973171</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -708,7 +736,7 @@
         <v>4577279</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -716,7 +744,7 @@
         <v>4584479</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -724,7 +752,7 @@
         <v>4616886</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -732,7 +760,7 @@
         <v>5098711</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -740,7 +768,7 @@
         <v>5098712</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -748,7 +776,7 @@
         <v>3248104</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -756,7 +784,7 @@
         <v>3273298</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -764,7 +792,7 @@
         <v>3284111</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -772,7 +800,7 @@
         <v>3330885</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -780,7 +808,7 @@
         <v>1045794</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -788,7 +816,7 @@
         <v>1009795</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -796,7 +824,7 @@
         <v>962997</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -804,7 +832,7 @@
         <v>941395</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -812,7 +840,7 @@
         <v>3877173</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -820,7 +848,7 @@
         <v>3884370</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -828,7 +856,7 @@
         <v>3880763</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -836,7 +864,7 @@
         <v>3170683</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -844,7 +872,7 @@
         <v>3152735</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -852,7 +880,7 @@
         <v>3152756</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -860,7 +888,7 @@
         <v>3145557</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -868,7 +896,7 @@
         <v>1927804</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -876,7 +904,7 @@
         <v>1909858</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -884,7 +912,7 @@
         <v>1873899</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -892,7 +920,7 @@
         <v>1899096</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -900,7 +928,7 @@
         <v>1891894</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -908,7 +936,7 @@
         <v>1935136</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -916,7 +944,7 @@
         <v>1949546</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -924,7 +952,7 @@
         <v>1942349</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -932,7 +960,7 @@
         <v>1658165</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -940,11 +968,12 @@
         <v>1632967</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>